<commit_message>
bayprotab ft dropdown added
</commit_message>
<xml_diff>
--- a/public/images/certificate/certificate.xlsx
+++ b/public/images/certificate/certificate.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t xml:space="preserve">SL</t>
   </si>
@@ -34,12 +34,6 @@
     <t xml:space="preserve">Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jayanti Rani</t>
   </si>
   <si>
@@ -47,12 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">CMES-JAL-0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/10/2021 to 22/12/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/03/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Purnima Rani</t>
@@ -208,19 +196,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,15 +224,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -253,9 +347,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="5" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -271,31 +364,19 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>10001</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,19 +384,13 @@
         <v>10002</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,18 +398,12 @@
         <v>10003</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -343,19 +412,13 @@
         <v>10004</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,19 +426,13 @@
         <v>10005</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,19 +440,13 @@
         <v>10006</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,19 +454,13 @@
         <v>10007</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,19 +468,13 @@
         <v>10008</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,19 +482,13 @@
         <v>10009</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,25 +496,19 @@
         <v>10010</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>